<commit_message>
Big overhaul: Removal of dummies. Added report section.
</commit_message>
<xml_diff>
--- a/Data/MY - GDPpC.xlsx
+++ b/Data/MY - GDPpC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\Dissertation\Migration\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757D8A27-896E-43E8-84F9-ED737EFD7C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377E181-55C1-40A2-88AE-012D48B03CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{80DCEE1E-7FA5-4145-A929-B3A5CAEE7105}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{80DCEE1E-7FA5-4145-A929-B3A5CAEE7105}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -455,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42B03E-A9D5-46ED-9D7A-CE574B776100}">
   <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +486,7 @@
       <c r="C2">
         <v>16762.059724349157</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -515,7 +514,7 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>2010</v>
       </c>
       <c r="C5">
@@ -526,7 +525,7 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>2011</v>
       </c>
       <c r="C6">
@@ -537,7 +536,7 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>2012</v>
       </c>
       <c r="C7">
@@ -548,7 +547,7 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>2013</v>
       </c>
       <c r="C8">
@@ -559,7 +558,7 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>2014</v>
       </c>
       <c r="C9">
@@ -570,7 +569,7 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>2015</v>
       </c>
       <c r="C10">
@@ -581,7 +580,7 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>2017</v>
       </c>
       <c r="C11">
@@ -592,7 +591,7 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>2019</v>
       </c>
       <c r="C12">
@@ -636,7 +635,7 @@
       <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>2010</v>
       </c>
       <c r="C16">
@@ -647,7 +646,7 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>2011</v>
       </c>
       <c r="C17">
@@ -658,7 +657,7 @@
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>2012</v>
       </c>
       <c r="C18">
@@ -669,7 +668,7 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>2013</v>
       </c>
       <c r="C19">
@@ -680,7 +679,7 @@
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>2014</v>
       </c>
       <c r="C20">
@@ -691,7 +690,7 @@
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>2015</v>
       </c>
       <c r="C21">
@@ -702,7 +701,7 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>2017</v>
       </c>
       <c r="C22">
@@ -713,7 +712,7 @@
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>2019</v>
       </c>
       <c r="C23">
@@ -757,7 +756,7 @@
       <c r="A27" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>2010</v>
       </c>
       <c r="C27">
@@ -768,7 +767,7 @@
       <c r="A28" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>2011</v>
       </c>
       <c r="C28">
@@ -779,7 +778,7 @@
       <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>2012</v>
       </c>
       <c r="C29">
@@ -790,7 +789,7 @@
       <c r="A30" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>2013</v>
       </c>
       <c r="C30">
@@ -801,7 +800,7 @@
       <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>2014</v>
       </c>
       <c r="C31">
@@ -812,7 +811,7 @@
       <c r="A32" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>2015</v>
       </c>
       <c r="C32">
@@ -823,7 +822,7 @@
       <c r="A33" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>2017</v>
       </c>
       <c r="C33">
@@ -834,7 +833,7 @@
       <c r="A34" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>2019</v>
       </c>
       <c r="C34">
@@ -878,7 +877,7 @@
       <c r="A38" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
         <v>2010</v>
       </c>
       <c r="C38">
@@ -889,7 +888,7 @@
       <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
         <v>2011</v>
       </c>
       <c r="C39">
@@ -900,7 +899,7 @@
       <c r="A40" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40">
         <v>2012</v>
       </c>
       <c r="C40">
@@ -911,7 +910,7 @@
       <c r="A41" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41">
         <v>2013</v>
       </c>
       <c r="C41">
@@ -922,7 +921,7 @@
       <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42">
         <v>2014</v>
       </c>
       <c r="C42">
@@ -933,7 +932,7 @@
       <c r="A43" t="s">
         <v>13</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43">
         <v>2015</v>
       </c>
       <c r="C43">
@@ -944,7 +943,7 @@
       <c r="A44" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44">
         <v>2017</v>
       </c>
       <c r="C44">
@@ -955,7 +954,7 @@
       <c r="A45" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45">
         <v>2019</v>
       </c>
       <c r="C45">
@@ -999,7 +998,7 @@
       <c r="A49" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49">
         <v>2010</v>
       </c>
       <c r="C49">
@@ -1010,7 +1009,7 @@
       <c r="A50" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50">
         <v>2011</v>
       </c>
       <c r="C50">
@@ -1021,7 +1020,7 @@
       <c r="A51" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51">
         <v>2012</v>
       </c>
       <c r="C51">
@@ -1032,7 +1031,7 @@
       <c r="A52" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52">
         <v>2013</v>
       </c>
       <c r="C52">
@@ -1043,7 +1042,7 @@
       <c r="A53" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53">
         <v>2014</v>
       </c>
       <c r="C53">
@@ -1054,7 +1053,7 @@
       <c r="A54" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54">
         <v>2015</v>
       </c>
       <c r="C54">
@@ -1065,7 +1064,7 @@
       <c r="A55" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55">
         <v>2017</v>
       </c>
       <c r="C55">
@@ -1076,7 +1075,7 @@
       <c r="A56" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56">
         <v>2019</v>
       </c>
       <c r="C56">
@@ -1120,7 +1119,7 @@
       <c r="A60" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60">
         <v>2010</v>
       </c>
       <c r="C60">
@@ -1131,7 +1130,7 @@
       <c r="A61" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
         <v>2011</v>
       </c>
       <c r="C61">
@@ -1142,7 +1141,7 @@
       <c r="A62" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62">
         <v>2012</v>
       </c>
       <c r="C62">
@@ -1153,7 +1152,7 @@
       <c r="A63" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63">
         <v>2013</v>
       </c>
       <c r="C63">
@@ -1164,7 +1163,7 @@
       <c r="A64" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64">
         <v>2014</v>
       </c>
       <c r="C64">
@@ -1175,7 +1174,7 @@
       <c r="A65" t="s">
         <v>3</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
         <v>2015</v>
       </c>
       <c r="C65">
@@ -1186,7 +1185,7 @@
       <c r="A66" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66">
         <v>2017</v>
       </c>
       <c r="C66">
@@ -1197,7 +1196,7 @@
       <c r="A67" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67">
         <v>2019</v>
       </c>
       <c r="C67">
@@ -1241,7 +1240,7 @@
       <c r="A71" t="s">
         <v>4</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
         <v>2010</v>
       </c>
       <c r="C71">
@@ -1252,7 +1251,7 @@
       <c r="A72" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72">
         <v>2011</v>
       </c>
       <c r="C72">
@@ -1263,7 +1262,7 @@
       <c r="A73" t="s">
         <v>4</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
         <v>2012</v>
       </c>
       <c r="C73">
@@ -1274,7 +1273,7 @@
       <c r="A74" t="s">
         <v>4</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74">
         <v>2013</v>
       </c>
       <c r="C74">
@@ -1285,7 +1284,7 @@
       <c r="A75" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75">
         <v>2014</v>
       </c>
       <c r="C75">
@@ -1296,7 +1295,7 @@
       <c r="A76" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76">
         <v>2015</v>
       </c>
       <c r="C76">
@@ -1307,7 +1306,7 @@
       <c r="A77" t="s">
         <v>4</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77">
         <v>2017</v>
       </c>
       <c r="C77">
@@ -1318,7 +1317,7 @@
       <c r="A78" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78">
         <v>2019</v>
       </c>
       <c r="C78">
@@ -1362,7 +1361,7 @@
       <c r="A82" t="s">
         <v>5</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82">
         <v>2010</v>
       </c>
       <c r="C82">
@@ -1373,7 +1372,7 @@
       <c r="A83" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83">
         <v>2011</v>
       </c>
       <c r="C83">
@@ -1384,7 +1383,7 @@
       <c r="A84" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84">
         <v>2012</v>
       </c>
       <c r="C84">
@@ -1395,7 +1394,7 @@
       <c r="A85" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85">
         <v>2013</v>
       </c>
       <c r="C85">
@@ -1406,7 +1405,7 @@
       <c r="A86" t="s">
         <v>5</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86">
         <v>2014</v>
       </c>
       <c r="C86">
@@ -1417,7 +1416,7 @@
       <c r="A87" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87">
         <v>2015</v>
       </c>
       <c r="C87">
@@ -1428,7 +1427,7 @@
       <c r="A88" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88">
         <v>2017</v>
       </c>
       <c r="C88">
@@ -1439,7 +1438,7 @@
       <c r="A89" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89">
         <v>2019</v>
       </c>
       <c r="C89">
@@ -1483,7 +1482,7 @@
       <c r="A93" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93">
         <v>2010</v>
       </c>
       <c r="C93">
@@ -1494,7 +1493,7 @@
       <c r="A94" t="s">
         <v>7</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94">
         <v>2011</v>
       </c>
       <c r="C94">
@@ -1505,7 +1504,7 @@
       <c r="A95" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95">
         <v>2012</v>
       </c>
       <c r="C95">
@@ -1516,7 +1515,7 @@
       <c r="A96" t="s">
         <v>7</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96">
         <v>2013</v>
       </c>
       <c r="C96">
@@ -1527,7 +1526,7 @@
       <c r="A97" t="s">
         <v>7</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97">
         <v>2014</v>
       </c>
       <c r="C97">
@@ -1538,7 +1537,7 @@
       <c r="A98" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98">
         <v>2015</v>
       </c>
       <c r="C98">
@@ -1549,7 +1548,7 @@
       <c r="A99" t="s">
         <v>7</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99">
         <v>2017</v>
       </c>
       <c r="C99">
@@ -1560,7 +1559,7 @@
       <c r="A100" t="s">
         <v>7</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100">
         <v>2019</v>
       </c>
       <c r="C100">
@@ -1604,7 +1603,7 @@
       <c r="A104" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104">
         <v>2010</v>
       </c>
       <c r="C104">
@@ -1615,7 +1614,7 @@
       <c r="A105" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105">
         <v>2011</v>
       </c>
       <c r="C105">
@@ -1626,7 +1625,7 @@
       <c r="A106" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106">
         <v>2012</v>
       </c>
       <c r="C106">
@@ -1637,7 +1636,7 @@
       <c r="A107" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107">
         <v>2013</v>
       </c>
       <c r="C107">
@@ -1648,7 +1647,7 @@
       <c r="A108" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108">
         <v>2014</v>
       </c>
       <c r="C108">
@@ -1659,7 +1658,7 @@
       <c r="A109" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109">
         <v>2015</v>
       </c>
       <c r="C109">
@@ -1670,7 +1669,7 @@
       <c r="A110" t="s">
         <v>8</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110">
         <v>2017</v>
       </c>
       <c r="C110">
@@ -1681,7 +1680,7 @@
       <c r="A111" t="s">
         <v>8</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111">
         <v>2019</v>
       </c>
       <c r="C111">
@@ -1725,7 +1724,7 @@
       <c r="A115" t="s">
         <v>6</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115">
         <v>2010</v>
       </c>
       <c r="C115">
@@ -1736,7 +1735,7 @@
       <c r="A116" t="s">
         <v>6</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116">
         <v>2011</v>
       </c>
       <c r="C116">
@@ -1747,7 +1746,7 @@
       <c r="A117" t="s">
         <v>6</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117">
         <v>2012</v>
       </c>
       <c r="C117">
@@ -1758,7 +1757,7 @@
       <c r="A118" t="s">
         <v>6</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118">
         <v>2013</v>
       </c>
       <c r="C118">
@@ -1769,7 +1768,7 @@
       <c r="A119" t="s">
         <v>6</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119">
         <v>2014</v>
       </c>
       <c r="C119">
@@ -1780,7 +1779,7 @@
       <c r="A120" t="s">
         <v>6</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120">
         <v>2015</v>
       </c>
       <c r="C120">
@@ -1791,7 +1790,7 @@
       <c r="A121" t="s">
         <v>6</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121">
         <v>2017</v>
       </c>
       <c r="C121">
@@ -1802,7 +1801,7 @@
       <c r="A122" t="s">
         <v>6</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122">
         <v>2019</v>
       </c>
       <c r="C122">
@@ -1846,7 +1845,7 @@
       <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126">
         <v>2010</v>
       </c>
       <c r="C126">
@@ -1857,7 +1856,7 @@
       <c r="A127" t="s">
         <v>11</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127">
         <v>2011</v>
       </c>
       <c r="C127">
@@ -1868,7 +1867,7 @@
       <c r="A128" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128">
         <v>2012</v>
       </c>
       <c r="C128">
@@ -1879,7 +1878,7 @@
       <c r="A129" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129">
         <v>2013</v>
       </c>
       <c r="C129">
@@ -1890,7 +1889,7 @@
       <c r="A130" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130">
         <v>2014</v>
       </c>
       <c r="C130">
@@ -1901,7 +1900,7 @@
       <c r="A131" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131">
         <v>2015</v>
       </c>
       <c r="C131">
@@ -1912,7 +1911,7 @@
       <c r="A132" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132">
         <v>2017</v>
       </c>
       <c r="C132">
@@ -1923,7 +1922,7 @@
       <c r="A133" t="s">
         <v>11</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B133">
         <v>2019</v>
       </c>
       <c r="C133">
@@ -1967,7 +1966,7 @@
       <c r="A137" t="s">
         <v>12</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137">
         <v>2010</v>
       </c>
       <c r="C137">
@@ -1978,7 +1977,7 @@
       <c r="A138" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138">
         <v>2011</v>
       </c>
       <c r="C138">
@@ -1989,7 +1988,7 @@
       <c r="A139" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139">
         <v>2012</v>
       </c>
       <c r="C139">
@@ -2000,7 +1999,7 @@
       <c r="A140" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="1">
+      <c r="B140">
         <v>2013</v>
       </c>
       <c r="C140">
@@ -2011,7 +2010,7 @@
       <c r="A141" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="1">
+      <c r="B141">
         <v>2014</v>
       </c>
       <c r="C141">
@@ -2022,7 +2021,7 @@
       <c r="A142" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B142">
         <v>2015</v>
       </c>
       <c r="C142">
@@ -2033,7 +2032,7 @@
       <c r="A143" t="s">
         <v>12</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143">
         <v>2017</v>
       </c>
       <c r="C143">
@@ -2044,7 +2043,7 @@
       <c r="A144" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="1">
+      <c r="B144">
         <v>2019</v>
       </c>
       <c r="C144">
@@ -2088,7 +2087,7 @@
       <c r="A148" t="s">
         <v>9</v>
       </c>
-      <c r="B148" s="1">
+      <c r="B148">
         <v>2010</v>
       </c>
       <c r="C148">
@@ -2099,7 +2098,7 @@
       <c r="A149" t="s">
         <v>9</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149">
         <v>2011</v>
       </c>
       <c r="C149">
@@ -2110,7 +2109,7 @@
       <c r="A150" t="s">
         <v>9</v>
       </c>
-      <c r="B150" s="1">
+      <c r="B150">
         <v>2012</v>
       </c>
       <c r="C150">
@@ -2121,7 +2120,7 @@
       <c r="A151" t="s">
         <v>9</v>
       </c>
-      <c r="B151" s="1">
+      <c r="B151">
         <v>2013</v>
       </c>
       <c r="C151">
@@ -2132,7 +2131,7 @@
       <c r="A152" t="s">
         <v>9</v>
       </c>
-      <c r="B152" s="1">
+      <c r="B152">
         <v>2014</v>
       </c>
       <c r="C152">
@@ -2143,7 +2142,7 @@
       <c r="A153" t="s">
         <v>9</v>
       </c>
-      <c r="B153" s="1">
+      <c r="B153">
         <v>2015</v>
       </c>
       <c r="C153">
@@ -2154,7 +2153,7 @@
       <c r="A154" t="s">
         <v>9</v>
       </c>
-      <c r="B154" s="1">
+      <c r="B154">
         <v>2017</v>
       </c>
       <c r="C154">
@@ -2165,7 +2164,7 @@
       <c r="A155" t="s">
         <v>9</v>
       </c>
-      <c r="B155" s="1">
+      <c r="B155">
         <v>2019</v>
       </c>
       <c r="C155">
@@ -2209,7 +2208,7 @@
       <c r="A159" t="s">
         <v>10</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159">
         <v>2010</v>
       </c>
       <c r="C159">
@@ -2220,7 +2219,7 @@
       <c r="A160" t="s">
         <v>10</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160">
         <v>2011</v>
       </c>
       <c r="C160">
@@ -2231,7 +2230,7 @@
       <c r="A161" t="s">
         <v>10</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161">
         <v>2012</v>
       </c>
       <c r="C161">
@@ -2242,7 +2241,7 @@
       <c r="A162" t="s">
         <v>10</v>
       </c>
-      <c r="B162" s="1">
+      <c r="B162">
         <v>2013</v>
       </c>
       <c r="C162">
@@ -2253,7 +2252,7 @@
       <c r="A163" t="s">
         <v>10</v>
       </c>
-      <c r="B163" s="1">
+      <c r="B163">
         <v>2014</v>
       </c>
       <c r="C163">
@@ -2264,7 +2263,7 @@
       <c r="A164" t="s">
         <v>10</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164">
         <v>2015</v>
       </c>
       <c r="C164">
@@ -2275,7 +2274,7 @@
       <c r="A165" t="s">
         <v>10</v>
       </c>
-      <c r="B165" s="1">
+      <c r="B165">
         <v>2017</v>
       </c>
       <c r="C165">
@@ -2286,7 +2285,7 @@
       <c r="A166" t="s">
         <v>10</v>
       </c>
-      <c r="B166" s="1">
+      <c r="B166">
         <v>2019</v>
       </c>
       <c r="C166">
@@ -2314,62 +2313,62 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>0.19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1.79</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>1.01</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>1.71</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>2.31</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>0.94</v>
       </c>
     </row>

</xml_diff>